<commit_message>
Starting one last test suite
</commit_message>
<xml_diff>
--- a/tests/Katalon_test_Centreon/Excel file/Premiere_automatisation_classeur.xlsx
+++ b/tests/Katalon_test_Centreon/Excel file/Premiere_automatisation_classeur.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgallardo\Desktop\Katalon\Katalon_Centreon\Excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27CFC63-BC6C-4745-AE64-7C1AAB339419}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F531BB-B13B-4F3E-BF5A-D2489CEC9AF0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="712" firstSheet="8" activeTab="9" xr2:uid="{FF50512E-4DF0-4DF5-91D6-9D6A0762A790}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="712" firstSheet="10" activeTab="11" xr2:uid="{FF50512E-4DF0-4DF5-91D6-9D6A0762A790}"/>
   </bookViews>
   <sheets>
     <sheet name="ACL action" sheetId="16" r:id="rId1"/>
@@ -23,18 +23,20 @@
     <sheet name="ACL menu Administration" sheetId="15" r:id="rId8"/>
     <sheet name="ACL resource" sheetId="18" r:id="rId9"/>
     <sheet name="Configuration" sheetId="17" r:id="rId10"/>
-    <sheet name="Host template" sheetId="1" r:id="rId11"/>
-    <sheet name="Host data" sheetId="2" r:id="rId12"/>
-    <sheet name="Host group" sheetId="7" r:id="rId13"/>
-    <sheet name="Meta service" sheetId="19" r:id="rId14"/>
-    <sheet name="Services" sheetId="4" r:id="rId15"/>
-    <sheet name="Service group" sheetId="8" r:id="rId16"/>
-    <sheet name="User config" sheetId="5" r:id="rId17"/>
-    <sheet name="Virtual metric" sheetId="20" r:id="rId18"/>
+    <sheet name="Contact group" sheetId="22" r:id="rId11"/>
+    <sheet name="Escalations" sheetId="23" r:id="rId12"/>
+    <sheet name="Host template" sheetId="1" r:id="rId13"/>
+    <sheet name="Host data" sheetId="2" r:id="rId14"/>
+    <sheet name="Host group" sheetId="7" r:id="rId15"/>
+    <sheet name="Meta service" sheetId="19" r:id="rId16"/>
+    <sheet name="Services" sheetId="4" r:id="rId17"/>
+    <sheet name="Service group" sheetId="8" r:id="rId18"/>
+    <sheet name="User config" sheetId="5" r:id="rId19"/>
+    <sheet name="Virtual metric" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="262">
   <si>
     <t>Host template</t>
   </si>
@@ -749,102 +751,92 @@
     <t>ServNotifOptions</t>
   </si>
   <si>
-    <t>20180905_105037</t>
-  </si>
-  <si>
-    <t>qNxTsj61</t>
-  </si>
-  <si>
-    <t>20180905_141803</t>
-  </si>
-  <si>
-    <t>20180905_142559</t>
-  </si>
-  <si>
-    <t>YjkHI7ajMq</t>
-  </si>
-  <si>
-    <t>20180905_145327</t>
-  </si>
-  <si>
-    <t>20180905_145643</t>
-  </si>
-  <si>
-    <t>20180905_150051</t>
-  </si>
-  <si>
-    <t>AlGy8g6Z</t>
-  </si>
-  <si>
-    <t>20180905_154809</t>
-  </si>
-  <si>
-    <t>xaZBCHSfc</t>
-  </si>
-  <si>
-    <t>20180905_162143</t>
-  </si>
-  <si>
-    <t>9ZvyMcM71G</t>
-  </si>
-  <si>
-    <t>20180905_165017</t>
-  </si>
-  <si>
-    <t>gAHH9agD</t>
-  </si>
-  <si>
-    <t>20180906_115519</t>
-  </si>
-  <si>
-    <t>i2CX9Y9N</t>
-  </si>
-  <si>
-    <t>20180906_134008</t>
-  </si>
-  <si>
-    <t>20180906_135304</t>
-  </si>
-  <si>
-    <t>20180906_153407</t>
-  </si>
-  <si>
-    <t>20180907_092408</t>
-  </si>
-  <si>
-    <t>AYxQeTR5U</t>
-  </si>
-  <si>
-    <t>20180907_101918</t>
-  </si>
-  <si>
-    <t>V2Eihs364</t>
-  </si>
-  <si>
-    <t>20180907_105300</t>
-  </si>
-  <si>
-    <t>IrixUi40</t>
-  </si>
-  <si>
-    <t>20180907_142516</t>
-  </si>
-  <si>
-    <t>phJ40BQR9</t>
-  </si>
-  <si>
     <t>20180907_143028</t>
   </si>
   <si>
-    <t>45f0iQ52</t>
+    <t>Escalation_user</t>
+  </si>
+  <si>
+    <t>Escalation_user_alias</t>
+  </si>
+  <si>
+    <t>escalation@localhost</t>
+  </si>
+  <si>
+    <t>Escalation_host</t>
+  </si>
+  <si>
+    <t>Escalation_host_alias</t>
+  </si>
+  <si>
+    <t>Recovery</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>workhours</t>
+  </si>
+  <si>
+    <t>cgName</t>
+  </si>
+  <si>
+    <t>cgAlias</t>
+  </si>
+  <si>
+    <t>esc_group</t>
+  </si>
+  <si>
+    <t>esc_group_alias</t>
+  </si>
+  <si>
+    <t>Flapping</t>
+  </si>
+  <si>
+    <t>kpcXqFxV79</t>
+  </si>
+  <si>
+    <t>escalationName</t>
+  </si>
+  <si>
+    <t>escalationAlias</t>
+  </si>
+  <si>
+    <t>firstNotif</t>
+  </si>
+  <si>
+    <t>lastNotif</t>
+  </si>
+  <si>
+    <t>notifInterval</t>
+  </si>
+  <si>
+    <t>escalation_alias1</t>
+  </si>
+  <si>
+    <t>Katalon_escalation1</t>
+  </si>
+  <si>
+    <t>Katalon_escalation2</t>
+  </si>
+  <si>
+    <t>escalation_alias2</t>
+  </si>
+  <si>
+    <t>serviceEscOptions</t>
+  </si>
+  <si>
+    <t>esc_group2</t>
+  </si>
+  <si>
+    <t>esc_group3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1208,7 +1200,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1235,14 +1227,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A79A66F-B8C9-414F-833E-0810106F2300}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,7 +1262,7 @@
         <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,6 +1280,139 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B534CD-8DB8-4CBD-A1D2-30123E54198E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDEB062-898A-419C-B2CD-941269A9D0D1}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3916544-D1B4-48DC-8947-EC28BCCD29FB}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1297,7 +1422,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.5703125" collapsed="true"/>
+    <col min="1" max="1" width="38.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1321,23 +1446,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BDF9CB-C323-4E14-A163-DB620EB7D4E1}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="8.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1409,12 +1534,35 @@
         <v>225</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AFB7E6D-0E7D-4321-AF2B-D50D514CFFE9}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1424,8 +1572,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1449,7 +1597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB4CC6B-7EDA-4E72-9EB5-BBA49468D440}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -1459,18 +1607,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1560,7 +1708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90314492-28ED-4CD2-BC3C-9965A9779B29}">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1570,7 +1718,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1653,7 +1801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86F19D1-89CE-44C5-B9CE-30DDC6FFCBE7}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1663,8 +1811,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="2" max="2" width="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1694,27 +1842,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DEBE12-2FF2-49B0-BBFA-62BAAF780BD8}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1787,60 +1935,54 @@
         <v>222</v>
       </c>
       <c r="K2" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="L2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I3" t="s">
+        <v>243</v>
+      </c>
+      <c r="J3" t="s">
+        <v>222</v>
+      </c>
+      <c r="L3" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4A3D0C26-D19C-4D8D-9C59-7EFB9EB36E84}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{164FCA5E-A193-49C4-A67F-D95332E620F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C65D18-01C1-480F-AFC4-B1DB4CE3C960}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.5703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1854,10 +1996,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1874,6 +2016,48 @@
       </c>
       <c r="B2" t="s">
         <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C65D18-01C1-480F-AFC4-B1DB4CE3C960}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -1891,34 +2075,34 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1952,19 +2136,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2064,27 +2248,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -2238,11 +2422,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2300,60 +2484,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="19" max="20" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="40" max="40" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="42" max="42" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="44" max="44" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="45" max="45" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="50" max="50" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="51" max="51" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="52" max="52" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="53" max="53" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="54" max="54" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="55" max="55" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="56" max="56" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="8.42578125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="8.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8.28515625" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="19" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="6" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="6.140625" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="28" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="26" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="12" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="16.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
@@ -2711,35 +2895,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="19" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -2947,8 +3131,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>